<commit_message>
Se procesan de nuevo los datos con las nuevas dimensiones curadas
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>tipo-vivienda</t>
   </si>
@@ -61,15 +61,9 @@
     <t>null</t>
   </si>
   <si>
-    <t>iaest-measure:municipio-nombre</t>
-  </si>
-  <si>
     <t>sdmx-dimension:refArea</t>
   </si>
   <si>
-    <t>iaest-dimension:aragon</t>
-  </si>
-  <si>
     <t>dim</t>
   </si>
   <si>
@@ -82,9 +76,15 @@
     <t>xsd:int</t>
   </si>
   <si>
+    <t>URI-Municipio</t>
+  </si>
+  <si>
     <t>URI-Provincia</t>
   </si>
   <si>
+    <t>URI-Comunidad</t>
+  </si>
+  <si>
     <t>URI-comarca</t>
   </si>
   <si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>mapping-clase-vivienda-detalle.xlsx</t>
-  </si>
-  <si>
-    <t>mapping-aragon.xlsx</t>
   </si>
 </sst>
 </file>
@@ -212,16 +209,16 @@
         <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
@@ -229,34 +226,34 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>15</v>
@@ -264,28 +261,28 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>15</v>
@@ -306,9 +303,6 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#8 Mejorar la generación de SKOS Concept Schemes #16 Incluir descripciones para algunas medidas en los DSDs #17 Referenciada codelist que luego no tiene valores #19 Añadir propiedad en el DSD que identifique el ámbito territorial aplicable #20 Generación errónea de medidas en 01-080101-010105TC
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
@@ -13,57 +13,57 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
-    <t>tipo-vivienda</t>
-  </si>
-  <si>
-    <t>total-viviendas</t>
-  </si>
-  <si>
-    <t>clase-vivienda-agregado</t>
-  </si>
-  <si>
-    <t>clase-vivienda-detalle</t>
-  </si>
-  <si>
-    <t>comarca-codigo</t>
-  </si>
-  <si>
-    <t>municipio-nombre</t>
-  </si>
-  <si>
-    <t>provincia-nombre</t>
-  </si>
-  <si>
-    <t>aragon</t>
-  </si>
-  <si>
-    <t>provincia-codigo</t>
-  </si>
-  <si>
-    <t>comarca-nombre</t>
-  </si>
-  <si>
-    <t>municipio-codigo</t>
+    <t>Tipo vivienda</t>
+  </si>
+  <si>
+    <t>Comarca nombre</t>
+  </si>
+  <si>
+    <t>Comarca código</t>
+  </si>
+  <si>
+    <t>Clase vivienda (agregado)</t>
+  </si>
+  <si>
+    <t>Provincia código</t>
+  </si>
+  <si>
+    <t>Aragón</t>
+  </si>
+  <si>
+    <t>Clase vivienda (detalle)</t>
+  </si>
+  <si>
+    <t>Total viviendas</t>
+  </si>
+  <si>
+    <t>Municipio código</t>
+  </si>
+  <si>
+    <t>Provincia nombre</t>
+  </si>
+  <si>
+    <t>Municipio nombre</t>
   </si>
   <si>
     <t>iaest-dimension:tipo-vivienda</t>
   </si>
   <si>
+    <t>sdmx-dimension:refArea</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>iaest-dimension:clase-vivienda-agregado</t>
+  </si>
+  <si>
+    <t>iaest-dimension:clase-vivienda-detalle</t>
+  </si>
+  <si>
     <t>iaest-measure:total-viviendas</t>
   </si>
   <si>
-    <t>iaest-dimension:clase-vivienda-agregado</t>
-  </si>
-  <si>
-    <t>iaest-dimension:clase-vivienda-detalle</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>sdmx-dimension:refArea</t>
-  </si>
-  <si>
     <t>dim</t>
   </si>
   <si>
@@ -73,19 +73,19 @@
     <t>skos:Concept</t>
   </si>
   <si>
+    <t>URI-comarca</t>
+  </si>
+  <si>
+    <t>URI-Comunidad</t>
+  </si>
+  <si>
     <t>xsd:int</t>
   </si>
   <si>
+    <t>URI-Provincia</t>
+  </si>
+  <si>
     <t>URI-Municipio</t>
-  </si>
-  <si>
-    <t>URI-Provincia</t>
-  </si>
-  <si>
-    <t>URI-Comunidad</t>
-  </si>
-  <si>
-    <t>URI-comarca</t>
   </si>
   <si>
     <t>mapping-tipo-vivienda.xlsx</t>
@@ -203,25 +203,25 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -229,34 +229,34 @@
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -267,41 +267,41 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización  automatica mar abr  6 17:33:39 CEST 2021
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010001-A-TC-TM-TP.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Tipo vivienda</t>
   </si>
@@ -130,6 +130,9 @@
     <t>URI-Municipio</t>
   </si>
   <si>
+    <t>xsd:uri</t>
+  </si>
+  <si>
     <t>mapping-tipo-vivienda.xlsx</t>
   </si>
   <si>
@@ -142,13 +145,10 @@
     <t>constante</t>
   </si>
   <si>
-    <t>&lt;http://reference.data.gov.uk/id/year/2001&gt;</t>
+    <t>&lt;http://reference.data.gov.uk/id/year/2016&gt;</t>
   </si>
   <si>
     <t>clase-vivienda</t>
-  </si>
-  <si>
-    <t>Clase vivienda</t>
   </si>
 </sst>
 </file>
@@ -188,29 +188,31 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -220,24 +222,16 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="25.14"/>
-    <col customWidth="1" min="2" max="2" width="23.14"/>
-    <col customWidth="1" min="4" max="4" width="19.43"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -425,17 +419,19 @@
       <c r="K5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L6" s="4"/>
     </row>
@@ -445,7 +441,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="L7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -453,8 +449,8 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="L8" s="5" t="s">
-        <v>43</v>
+      <c r="L8" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -467,19 +463,11 @@
     </row>
     <row r="10">
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="1" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>